<commit_message>
Initial work getting the optimizer working again
</commit_message>
<xml_diff>
--- a/data/GroupSpec.xlsx
+++ b/data/GroupSpec.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DWMoreau/MLI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A994559-93CC-6940-8F5F-1CDFDB859897}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F31206-D887-0940-86B3-F371434F957E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="-19740" windowWidth="24700" windowHeight="17960" activeTab="2" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
+    <workbookView xWindow="1840" yWindow="1000" windowWidth="24700" windowHeight="17960" activeTab="3" xr2:uid="{7928E02C-29DC-574B-8667-D82DDE3DF551}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Groups V2" sheetId="2" r:id="rId2"/>
     <sheet name="Groups V3" sheetId="3" r:id="rId3"/>
+    <sheet name="Groups V3 Assessment" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4655" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4667" uniqueCount="292">
   <si>
     <t>spacegroup number</t>
   </si>
@@ -846,6 +847,63 @@
   </si>
   <si>
     <t>ortho_14</t>
+  </si>
+  <si>
+    <t>ortho_00</t>
+  </si>
+  <si>
+    <t>ortho_01</t>
+  </si>
+  <si>
+    <t>ortho_02</t>
+  </si>
+  <si>
+    <t>ortho_03</t>
+  </si>
+  <si>
+    <t>ortho_04</t>
+  </si>
+  <si>
+    <t>ortho_05</t>
+  </si>
+  <si>
+    <t>ortho_06</t>
+  </si>
+  <si>
+    <t>ortho_07</t>
+  </si>
+  <si>
+    <t>ortho_08</t>
+  </si>
+  <si>
+    <t>ortho_09</t>
+  </si>
+  <si>
+    <t>RMSE / 50% / 75%</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>loss</t>
   </si>
 </sst>
 </file>
@@ -7977,7 +8035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA753F3D-C6B3-CF4C-AC0A-0702F927E144}">
   <dimension ref="A1:K228"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A211" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A184" sqref="A184:XFD184"/>
     </sheetView>
   </sheetViews>
@@ -14751,8 +14809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D154C47-0A69-1C46-8595-34C42B00C9A5}">
   <dimension ref="A1:K257"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14813,7 +14871,7 @@
         <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="D3">
         <v>852</v>
@@ -14845,7 +14903,7 @@
         <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="D4">
         <v>2060</v>
@@ -14877,7 +14935,7 @@
         <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="D5">
         <v>127</v>
@@ -14909,7 +14967,7 @@
         <v>220</v>
       </c>
       <c r="C6" t="s">
-        <v>250</v>
+        <v>273</v>
       </c>
       <c r="D6">
         <v>844</v>
@@ -14947,7 +15005,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D9">
         <v>235</v>
@@ -14970,7 +15028,7 @@
         <v>267</v>
       </c>
       <c r="C10" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -14993,7 +15051,7 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D11">
         <v>67</v>
@@ -15016,7 +15074,7 @@
         <v>221</v>
       </c>
       <c r="C12" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D12">
         <v>205</v>
@@ -15039,7 +15097,7 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D13">
         <v>9618</v>
@@ -15062,7 +15120,7 @@
         <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D14">
         <v>91</v>
@@ -15085,7 +15143,7 @@
         <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D15">
         <v>258</v>
@@ -15108,7 +15166,7 @@
         <v>73</v>
       </c>
       <c r="C16" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D16">
         <v>153</v>
@@ -15131,7 +15189,7 @@
         <v>170</v>
       </c>
       <c r="C17" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D17">
         <v>254</v>
@@ -15154,7 +15212,7 @@
         <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D18">
         <v>42</v>
@@ -15177,7 +15235,7 @@
         <v>171</v>
       </c>
       <c r="C19" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D19">
         <v>256</v>
@@ -15200,7 +15258,7 @@
         <v>126</v>
       </c>
       <c r="C20" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D20">
         <v>80</v>
@@ -15223,7 +15281,7 @@
         <v>266</v>
       </c>
       <c r="C21" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -15246,7 +15304,7 @@
         <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>251</v>
+        <v>274</v>
       </c>
       <c r="D22">
         <v>70</v>
@@ -15276,7 +15334,7 @@
         <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -15302,7 +15360,7 @@
         <v>229</v>
       </c>
       <c r="C26" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D26">
         <v>103</v>
@@ -15328,7 +15386,7 @@
         <v>122</v>
       </c>
       <c r="C27" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D27">
         <v>25</v>
@@ -15354,7 +15412,7 @@
         <v>228</v>
       </c>
       <c r="C28" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D28">
         <v>15</v>
@@ -15380,7 +15438,7 @@
         <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D29">
         <v>2382</v>
@@ -15406,7 +15464,7 @@
         <v>185</v>
       </c>
       <c r="C30" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D30">
         <v>1595</v>
@@ -15432,7 +15490,7 @@
         <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D31">
         <v>121</v>
@@ -15458,7 +15516,7 @@
         <v>144</v>
       </c>
       <c r="C32" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D32">
         <v>259</v>
@@ -15484,7 +15542,7 @@
         <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D33">
         <v>2382</v>
@@ -15510,7 +15568,7 @@
         <v>186</v>
       </c>
       <c r="C34" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="D34">
         <v>2539</v>
@@ -15542,7 +15600,7 @@
         <v>124</v>
       </c>
       <c r="C37" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D37">
         <v>49</v>
@@ -15568,7 +15626,7 @@
         <v>116</v>
       </c>
       <c r="C38" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D38">
         <v>75</v>
@@ -15594,7 +15652,7 @@
         <v>119</v>
       </c>
       <c r="C39" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D39">
         <v>7</v>
@@ -15620,7 +15678,7 @@
         <v>231</v>
       </c>
       <c r="C40" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D40">
         <v>39</v>
@@ -15646,7 +15704,7 @@
         <v>226</v>
       </c>
       <c r="C41" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D41">
         <v>69</v>
@@ -15672,7 +15730,7 @@
         <v>188</v>
       </c>
       <c r="C42" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D42">
         <v>2308</v>
@@ -15698,7 +15756,7 @@
         <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D43">
         <v>296</v>
@@ -15724,7 +15782,7 @@
         <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D44">
         <v>2821</v>
@@ -15750,7 +15808,7 @@
         <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D45">
         <v>846</v>
@@ -15776,7 +15834,7 @@
         <v>183</v>
       </c>
       <c r="C46" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D46">
         <v>1380</v>
@@ -15802,7 +15860,7 @@
         <v>140</v>
       </c>
       <c r="C47" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="D47">
         <v>241</v>
@@ -15834,7 +15892,7 @@
         <v>230</v>
       </c>
       <c r="C50" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D50">
         <v>51</v>
@@ -15860,7 +15918,7 @@
         <v>227</v>
       </c>
       <c r="C51" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D51">
         <v>33</v>
@@ -15886,7 +15944,7 @@
         <v>123</v>
       </c>
       <c r="C52" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D52">
         <v>31</v>
@@ -15912,7 +15970,7 @@
         <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D53">
         <v>320</v>
@@ -15938,7 +15996,7 @@
         <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D54">
         <v>25</v>
@@ -15964,7 +16022,7 @@
         <v>67</v>
       </c>
       <c r="C55" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D55">
         <v>1064</v>
@@ -15990,7 +16048,7 @@
         <v>184</v>
       </c>
       <c r="C56" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D56">
         <v>1083</v>
@@ -16016,7 +16074,7 @@
         <v>139</v>
       </c>
       <c r="C57" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D57">
         <v>129</v>
@@ -16042,7 +16100,7 @@
         <v>141</v>
       </c>
       <c r="C58" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D58">
         <v>90</v>
@@ -16068,7 +16126,7 @@
         <v>70</v>
       </c>
       <c r="C59" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D59">
         <v>3384</v>
@@ -16094,7 +16152,7 @@
         <v>187</v>
       </c>
       <c r="C60" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="D60">
         <v>1243</v>
@@ -16126,7 +16184,7 @@
         <v>222</v>
       </c>
       <c r="C63" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D63">
         <v>140</v>
@@ -16155,7 +16213,7 @@
         <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D64">
         <v>12</v>
@@ -16184,7 +16242,7 @@
         <v>204</v>
       </c>
       <c r="C65" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D65">
         <v>52</v>
@@ -16213,7 +16271,7 @@
         <v>101</v>
       </c>
       <c r="C66" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D66">
         <v>78</v>
@@ -16242,7 +16300,7 @@
         <v>80</v>
       </c>
       <c r="C67" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D67">
         <v>153</v>
@@ -16271,7 +16329,7 @@
         <v>190</v>
       </c>
       <c r="C68" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D68">
         <v>155</v>
@@ -16300,7 +16358,7 @@
         <v>99</v>
       </c>
       <c r="C69" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D69">
         <v>68</v>
@@ -16329,7 +16387,7 @@
         <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D70">
         <v>118</v>
@@ -16358,7 +16416,7 @@
         <v>189</v>
       </c>
       <c r="C71" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D71">
         <v>179</v>
@@ -16387,7 +16445,7 @@
         <v>177</v>
       </c>
       <c r="C72" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D72">
         <v>2051</v>
@@ -16416,7 +16474,7 @@
         <v>160</v>
       </c>
       <c r="C73" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D73">
         <v>932</v>
@@ -16445,7 +16503,7 @@
         <v>175</v>
       </c>
       <c r="C74" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D74">
         <v>1357</v>
@@ -16474,7 +16532,7 @@
         <v>17</v>
       </c>
       <c r="C75" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="D75">
         <v>946</v>
@@ -16509,7 +16567,7 @@
         <v>223</v>
       </c>
       <c r="C78" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D78">
         <v>132</v>
@@ -16538,7 +16596,7 @@
         <v>85</v>
       </c>
       <c r="C79" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D79">
         <v>88</v>
@@ -16567,7 +16625,7 @@
         <v>205</v>
       </c>
       <c r="C80" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D80">
         <v>77</v>
@@ -16596,7 +16654,7 @@
         <v>81</v>
       </c>
       <c r="C81" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D81">
         <v>201</v>
@@ -16625,7 +16683,7 @@
         <v>102</v>
       </c>
       <c r="C82" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D82">
         <v>4</v>
@@ -16654,7 +16712,7 @@
         <v>192</v>
       </c>
       <c r="C83" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D83">
         <v>230</v>
@@ -16683,7 +16741,7 @@
         <v>100</v>
       </c>
       <c r="C84" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D84">
         <v>19</v>
@@ -16712,7 +16770,7 @@
         <v>79</v>
       </c>
       <c r="C85" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D85">
         <v>237</v>
@@ -16741,7 +16799,7 @@
         <v>191</v>
       </c>
       <c r="C86" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D86">
         <v>268</v>
@@ -16770,7 +16828,7 @@
         <v>18</v>
       </c>
       <c r="C87" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D87">
         <v>710</v>
@@ -16799,7 +16857,7 @@
         <v>178</v>
       </c>
       <c r="C88" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D88">
         <v>777</v>
@@ -16828,7 +16886,7 @@
         <v>161</v>
       </c>
       <c r="C89" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D89">
         <v>1326</v>
@@ -16857,7 +16915,7 @@
         <v>176</v>
       </c>
       <c r="C90" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D90">
         <v>946</v>
@@ -16893,7 +16951,7 @@
         <v>118</v>
       </c>
       <c r="C93" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D93">
         <v>170</v>
@@ -16922,7 +16980,7 @@
         <v>224</v>
       </c>
       <c r="C94" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D94">
         <v>117</v>
@@ -16951,7 +17009,7 @@
         <v>86</v>
       </c>
       <c r="C95" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D95">
         <v>9</v>
@@ -16980,7 +17038,7 @@
         <v>206</v>
       </c>
       <c r="C96" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D96">
         <v>23</v>
@@ -17009,7 +17067,7 @@
         <v>83</v>
       </c>
       <c r="C97" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D97">
         <v>427</v>
@@ -17038,7 +17096,7 @@
         <v>199</v>
       </c>
       <c r="C98" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D98">
         <v>205</v>
@@ -17067,7 +17125,7 @@
         <v>104</v>
       </c>
       <c r="C99" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D99">
         <v>15</v>
@@ -17096,7 +17154,7 @@
         <v>194</v>
       </c>
       <c r="C100" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D100">
         <v>126</v>
@@ -17125,7 +17183,7 @@
         <v>196</v>
       </c>
       <c r="C101" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D101">
         <v>126</v>
@@ -17154,7 +17212,7 @@
         <v>82</v>
       </c>
       <c r="C102" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D102">
         <v>211</v>
@@ -17183,7 +17241,7 @@
         <v>200</v>
       </c>
       <c r="C103" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D103">
         <v>240</v>
@@ -17212,7 +17270,7 @@
         <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D104">
         <v>13</v>
@@ -17241,7 +17299,7 @@
         <v>193</v>
       </c>
       <c r="C105" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D105">
         <v>117</v>
@@ -17270,7 +17328,7 @@
         <v>162</v>
       </c>
       <c r="C106" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D106">
         <v>1193</v>
@@ -17299,7 +17357,7 @@
         <v>180</v>
       </c>
       <c r="C107" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D107">
         <v>1100</v>
@@ -17328,7 +17386,7 @@
         <v>179</v>
       </c>
       <c r="C108" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D108">
         <v>2079</v>
@@ -17357,7 +17415,7 @@
         <v>19</v>
       </c>
       <c r="C109" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="D109">
         <v>70</v>
@@ -17392,7 +17450,7 @@
         <v>23</v>
       </c>
       <c r="C112" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D112">
         <v>36</v>
@@ -17424,7 +17482,7 @@
         <v>265</v>
       </c>
       <c r="C113" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D113">
         <v>2</v>
@@ -17456,7 +17514,7 @@
         <v>264</v>
       </c>
       <c r="C114" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D114">
         <v>6</v>
@@ -17488,7 +17546,7 @@
         <v>111</v>
       </c>
       <c r="C115" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D115">
         <v>71</v>
@@ -17520,7 +17578,7 @@
         <v>219</v>
       </c>
       <c r="C116" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D116">
         <v>98</v>
@@ -17552,7 +17610,7 @@
         <v>225</v>
       </c>
       <c r="C117" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D117">
         <v>268</v>
@@ -17584,7 +17642,7 @@
         <v>268</v>
       </c>
       <c r="C118" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D118">
         <v>3</v>
@@ -17616,7 +17674,7 @@
         <v>217</v>
       </c>
       <c r="C119" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D119">
         <v>16</v>
@@ -17648,7 +17706,7 @@
         <v>218</v>
       </c>
       <c r="C120" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D120">
         <v>16</v>
@@ -17680,7 +17738,7 @@
         <v>215</v>
       </c>
       <c r="C121" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D121">
         <v>85</v>
@@ -17712,7 +17770,7 @@
         <v>213</v>
       </c>
       <c r="C122" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D122">
         <v>8</v>
@@ -17744,7 +17802,7 @@
         <v>216</v>
       </c>
       <c r="C123" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D123">
         <v>123</v>
@@ -17776,7 +17834,7 @@
         <v>214</v>
       </c>
       <c r="C124" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D124">
         <v>161</v>
@@ -17808,7 +17866,7 @@
         <v>109</v>
       </c>
       <c r="C125" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D125">
         <v>89</v>
@@ -17840,7 +17898,7 @@
         <v>110</v>
       </c>
       <c r="C126" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D126">
         <v>122</v>
@@ -17872,7 +17930,7 @@
         <v>105</v>
       </c>
       <c r="C127" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D127">
         <v>343</v>
@@ -17904,7 +17962,7 @@
         <v>108</v>
       </c>
       <c r="C128" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D128">
         <v>126</v>
@@ -17936,7 +17994,7 @@
         <v>107</v>
       </c>
       <c r="C129" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D129">
         <v>272</v>
@@ -17968,7 +18026,7 @@
         <v>106</v>
       </c>
       <c r="C130" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D130">
         <v>70</v>
@@ -18000,7 +18058,7 @@
         <v>198</v>
       </c>
       <c r="C131" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D131">
         <v>205</v>
@@ -18032,7 +18090,7 @@
         <v>195</v>
       </c>
       <c r="C132" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D132">
         <v>208</v>
@@ -18064,7 +18122,7 @@
         <v>197</v>
       </c>
       <c r="C133" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="D133">
         <v>188</v>
@@ -18096,7 +18154,7 @@
         <v>181</v>
       </c>
       <c r="C136" t="s">
-        <v>259</v>
+        <v>282</v>
       </c>
       <c r="D136">
         <v>9742</v>
@@ -20777,4 +20835,61 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3F9838-AFC0-3642-9763-37608F10FBE8}">
+  <dimension ref="A2:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F4" t="s">
+        <v>288</v>
+      </c>
+      <c r="G4" t="s">
+        <v>287</v>
+      </c>
+      <c r="H4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>